<commit_message>
Modified biomass code is bad
</commit_message>
<xml_diff>
--- a/Experimental Results/cell dry weight measurements.xlsx
+++ b/Experimental Results/cell dry weight measurements.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="132" windowWidth="14340" windowHeight="5832"/>
+    <workbookView xWindow="390" yWindow="135" windowWidth="14340" windowHeight="5835"/>
   </bookViews>
   <sheets>
     <sheet name="Trial 1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="15">
   <si>
     <t xml:space="preserve">Date: </t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Density</t>
+  </si>
+  <si>
+    <t>OD = 1</t>
   </si>
 </sst>
 </file>
@@ -397,23 +400,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -427,7 +430,7 @@
         <v>0.89500000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -450,7 +453,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -476,7 +479,7 @@
         <v>0.61999999999997613</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -502,7 +505,7 @@
         <v>0.64000000000000057</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -528,7 +531,7 @@
         <v>0.70000000000000284</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>4</v>
       </c>
@@ -554,7 +557,7 @@
         <v>0.79999999999998295</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -582,8 +585,11 @@
         <f t="shared" si="3"/>
         <v>0.68999999999999062</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -611,8 +617,12 @@
         <f t="shared" ref="G9" si="5">STDEV(G4:G7)</f>
         <v>8.082903768654727E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I9">
+        <f>0.69/0.895</f>
+        <v>0.77094972067039103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -632,6 +642,9 @@
         <v>11</v>
       </c>
       <c r="G10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" t="s">
         <v>12</v>
       </c>
     </row>
@@ -648,14 +661,14 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -879,7 +892,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Took out dead ends from model. 4_14 is last
</commit_message>
<xml_diff>
--- a/Experimental Results/cell dry weight measurements.xlsx
+++ b/Experimental Results/cell dry weight measurements.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="135" windowWidth="14340" windowHeight="5835"/>
+    <workbookView xWindow="396" yWindow="132" windowWidth="14340" windowHeight="5832"/>
   </bookViews>
   <sheets>
     <sheet name="Trial 1" sheetId="1" r:id="rId1"/>
     <sheet name="Trial 2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Salts Calculations" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="34">
   <si>
     <t xml:space="preserve">Date: </t>
   </si>
@@ -61,6 +61,63 @@
   </si>
   <si>
     <t>OD = 1</t>
+  </si>
+  <si>
+    <t>Dry Wt. 2</t>
+  </si>
+  <si>
+    <t>Dry cell Wt. 2</t>
+  </si>
+  <si>
+    <t>Density 2</t>
+  </si>
+  <si>
+    <t>Compound</t>
+  </si>
+  <si>
+    <t>Amount (g)</t>
+  </si>
+  <si>
+    <t>KCl</t>
+  </si>
+  <si>
+    <t>NaCl</t>
+  </si>
+  <si>
+    <t>NaHCO3</t>
+  </si>
+  <si>
+    <t>FeSO4</t>
+  </si>
+  <si>
+    <t>CaCl2</t>
+  </si>
+  <si>
+    <t>MgCl2</t>
+  </si>
+  <si>
+    <t>MgSO4</t>
+  </si>
+  <si>
+    <t>Amount (mL)</t>
+  </si>
+  <si>
+    <t>Total Wt</t>
+  </si>
+  <si>
+    <t>g salts/g media</t>
+  </si>
+  <si>
+    <t>g salts in media</t>
+  </si>
+  <si>
+    <t>Wet-Dry</t>
+  </si>
+  <si>
+    <t>Minus Salts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Salt Density </t>
   </si>
 </sst>
 </file>
@@ -84,7 +141,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -92,13 +149,55 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,23 +499,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -430,7 +533,7 @@
         <v>0.89500000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -452,8 +555,26 @@
       <c r="G3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -478,8 +599,27 @@
         <f>F4/0.05</f>
         <v>0.61999999999997613</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K4">
+        <v>13.116</v>
+      </c>
+      <c r="L4">
+        <f>K4-B4</f>
+        <v>1.7999999999998906E-2</v>
+      </c>
+      <c r="M4">
+        <f>L4/0.05</f>
+        <v>0.35999999999997812</v>
+      </c>
+      <c r="N4">
+        <f>L4-'Salts Calculations'!D14*'Trial 1'!P4</f>
+        <v>1.7999999999998906E-2</v>
+      </c>
+      <c r="O4">
+        <f>N4/0.05</f>
+        <v>0.35999999999997812</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -504,8 +644,31 @@
         <f t="shared" ref="G5:G7" si="2">F5/0.05</f>
         <v>0.64000000000000057</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K5">
+        <v>13.129</v>
+      </c>
+      <c r="L5">
+        <f t="shared" ref="L5:L7" si="3">K5-B5</f>
+        <v>1.9000000000000128E-2</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ref="M5:M7" si="4">L5/0.05</f>
+        <v>0.38000000000000256</v>
+      </c>
+      <c r="N5">
+        <f>L5-'Salts Calculations'!D14*'Trial 1'!P5</f>
+        <v>2.3988513495995373E-3</v>
+      </c>
+      <c r="O5">
+        <f t="shared" ref="O5:O7" si="5">N5/0.05</f>
+        <v>4.7977026991990745E-2</v>
+      </c>
+      <c r="P5">
+        <f t="shared" ref="P5:P7" si="6">C5-K5</f>
+        <v>0.50699999999999967</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -530,8 +693,31 @@
         <f t="shared" si="2"/>
         <v>0.70000000000000284</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K6">
+        <v>13.096</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="3"/>
+        <v>2.2000000000000242E-2</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="4"/>
+        <v>0.44000000000000483</v>
+      </c>
+      <c r="N6">
+        <f>L6-'Salts Calculations'!D14*'Trial 1'!P6</f>
+        <v>2.2554385873936184E-3</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="5"/>
+        <v>4.5108771747872367E-2</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="6"/>
+        <v>0.60299999999999976</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>4</v>
       </c>
@@ -556,8 +742,31 @@
         <f t="shared" si="2"/>
         <v>0.79999999999998295</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K7">
+        <v>13.129</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="3"/>
+        <v>2.7999999999998693E-2</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="4"/>
+        <v>0.55999999999997385</v>
+      </c>
+      <c r="N7">
+        <f>L7-'Salts Calculations'!D14*'Trial 1'!P7</f>
+        <v>3.5075755611433321E-3</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="5"/>
+        <v>7.0151511222866642E-2</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="6"/>
+        <v>0.74800000000000111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -566,30 +775,46 @@
         <v>13.095749999999999</v>
       </c>
       <c r="C8">
-        <f t="shared" ref="C8:G8" si="3">AVERAGE(C4:C7)</f>
+        <f t="shared" ref="C8:G8" si="7">AVERAGE(C4:C7)</f>
         <v>13.71325</v>
       </c>
       <c r="D8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>13.13025</v>
       </c>
       <c r="E8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0.61749999999999972</v>
       </c>
       <c r="F8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>3.4499999999999531E-2</v>
       </c>
       <c r="G8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0.68999999999999062</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J8" s="5"/>
+      <c r="K8">
+        <f t="shared" ref="K8:M8" si="8">AVERAGE(K4:K7)</f>
+        <v>13.117499999999998</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="8"/>
+        <v>2.1749999999999492E-2</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="8"/>
+        <v>0.43499999999998984</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -598,31 +823,48 @@
         <v>1.5370426148939432E-2</v>
       </c>
       <c r="C9">
-        <f t="shared" ref="C9:F9" si="4">STDEV(C4:C7)</f>
+        <f t="shared" ref="C9:F9" si="9">STDEV(C4:C7)</f>
         <v>0.11284908801876416</v>
       </c>
       <c r="D9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>1.5348724159790278E-2</v>
       </c>
       <c r="E9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.11416508514719675</v>
       </c>
       <c r="F9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>4.0414518843273385E-3</v>
       </c>
       <c r="G9">
-        <f t="shared" ref="G9" si="5">STDEV(G4:G7)</f>
+        <f t="shared" ref="G9" si="10">STDEV(G4:G7)</f>
         <v>8.082903768654727E-2</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="3">
         <f>0.69/0.895</f>
         <v>0.77094972067039103</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J9" s="5"/>
+      <c r="K9">
+        <f t="shared" ref="K9:M9" si="11">STDEV(K4:K7)</f>
+        <v>1.558845726811965E-2</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="11"/>
+        <v>4.499999999999677E-3</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="11"/>
+        <v>8.9999999999993807E-2</v>
+      </c>
+      <c r="O9" s="3">
+        <f>M8/D1</f>
+        <v>0.48603351955306129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -644,7 +886,40 @@
       <c r="G10" t="s">
         <v>12</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="5"/>
+      <c r="K10" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10" t="s">
+        <v>11</v>
+      </c>
+      <c r="M10" t="s">
+        <v>12</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="P10" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E13">
+        <f>C8-K8</f>
+        <v>0.59575000000000244</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O16">
+        <f>AVERAGE(O4:O7)</f>
+        <v>0.13080932749067697</v>
+      </c>
+    </row>
+    <row r="17" spans="15:15" x14ac:dyDescent="0.3">
+      <c r="O17" t="s">
         <v>12</v>
       </c>
     </row>
@@ -655,23 +930,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -685,7 +961,7 @@
         <v>0.91500000000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -707,8 +983,17 @@
       <c r="G3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="K3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="15" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -730,8 +1015,19 @@
         <f>F4/0.05</f>
         <v>-262.44</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="K4">
+        <v>13.116</v>
+      </c>
+      <c r="L4">
+        <f>K4-B4</f>
+        <v>-6.0000000000002274E-3</v>
+      </c>
+      <c r="M4">
+        <f>L4/0.05</f>
+        <v>-0.12000000000000455</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="15" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -753,8 +1049,19 @@
         <f t="shared" ref="G5:G7" si="2">F5/0.05</f>
         <v>-261.88</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="K5">
+        <v>13.129</v>
+      </c>
+      <c r="L5">
+        <f t="shared" ref="L5:L7" si="3">K5-B5</f>
+        <v>3.5000000000000142E-2</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ref="M5:M7" si="4">L5/0.05</f>
+        <v>0.70000000000000284</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -776,8 +1083,19 @@
         <f t="shared" si="2"/>
         <v>-261.08</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="K6">
+        <v>13.096</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="3"/>
+        <v>4.1999999999999815E-2</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="4"/>
+        <v>0.83999999999999631</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>4</v>
       </c>
@@ -799,8 +1117,19 @@
         <f t="shared" si="2"/>
         <v>-262.15999999999997</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="K7">
+        <v>13.129</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="3"/>
+        <v>2.0999999999999019E-2</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="4"/>
+        <v>0.41999999999998039</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -809,27 +1138,46 @@
         <v>13.0945</v>
       </c>
       <c r="C8">
-        <f t="shared" ref="C8:G8" si="3">AVERAGE(C4:C7)</f>
+        <f t="shared" ref="C8:G8" si="5">AVERAGE(C4:C7)</f>
         <v>14.822749999999999</v>
       </c>
       <c r="D8" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.7282499999999996</v>
       </c>
       <c r="F8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-13.0945</v>
       </c>
       <c r="G8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-261.89</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="5"/>
+      <c r="K8">
+        <f t="shared" ref="K8:M8" si="6">AVERAGE(K4:K7)</f>
+        <v>13.117499999999998</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="6"/>
+        <v>2.2999999999999687E-2</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="6"/>
+        <v>0.45999999999999375</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -838,27 +1186,48 @@
         <v>2.9320072760255257E-2</v>
       </c>
       <c r="C9">
-        <f t="shared" ref="C9:G9" si="4">STDEV(C4:C7)</f>
+        <f t="shared" ref="C9:G9" si="7">STDEV(C4:C7)</f>
         <v>0.99476642987185615</v>
       </c>
       <c r="D9" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1.0029494420624259</v>
       </c>
       <c r="F9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>2.9320072760255257E-2</v>
       </c>
       <c r="G9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.58640145520510834</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I9" s="3">
+        <f>G8/D1</f>
+        <v>-286.21857923497265</v>
+      </c>
+      <c r="J9" s="5"/>
+      <c r="K9">
+        <f t="shared" ref="K9:M9" si="8">STDEV(K4:K7)</f>
+        <v>1.558845726811965E-2</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="8"/>
+        <v>2.1213203435596531E-2</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="8"/>
+        <v>0.42426406871193062</v>
+      </c>
+      <c r="O9" s="3">
+        <f>M8/D1</f>
+        <v>0.50273224043715159</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -878,6 +1247,22 @@
         <v>11</v>
       </c>
       <c r="G10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="5"/>
+      <c r="K10" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10" t="s">
+        <v>11</v>
+      </c>
+      <c r="M10" t="s">
+        <v>12</v>
+      </c>
+      <c r="O10" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -888,12 +1273,124 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>3.02</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6">
+        <v>24.75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7">
+        <v>31.05</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11">
+        <v>45</v>
+      </c>
+      <c r="H11">
+        <f>0.6*D14</f>
+        <v>1.9646329763787693E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D13">
+        <f>303/9000</f>
+        <v>3.3666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D14">
+        <f>B15/(B15+8953)</f>
+        <v>3.2743882939646154E-2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15">
+        <f>SUM(B2:B7)</f>
+        <v>303.08</v>
+      </c>
+      <c r="D15">
+        <f>1000*D14</f>
+        <v>32.743882939646156</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated model and calculations
</commit_message>
<xml_diff>
--- a/Experimental Results/cell dry weight measurements.xlsx
+++ b/Experimental Results/cell dry weight measurements.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="396" yWindow="132" windowWidth="14340" windowHeight="5832" activeTab="3"/>
+    <workbookView xWindow="390" yWindow="135" windowWidth="14340" windowHeight="5835" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Trial 1" sheetId="1" r:id="rId1"/>
@@ -342,11 +342,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="47190016"/>
-        <c:axId val="47188224"/>
+        <c:axId val="44600320"/>
+        <c:axId val="44606208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="47190016"/>
+        <c:axId val="44600320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -356,12 +356,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47188224"/>
+        <c:crossAx val="44606208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="47188224"/>
+        <c:axId val="44606208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -372,7 +372,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47190016"/>
+        <c:crossAx val="44600320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -717,21 +717,21 @@
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -745,7 +745,7 @@
         <v>0.89500000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -786,7 +786,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -831,7 +831,7 @@
         <v>0.35999999999997812</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -880,7 +880,7 @@
         <v>0.50699999999999967</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -929,7 +929,7 @@
         <v>0.60299999999999976</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>4</v>
       </c>
@@ -978,7 +978,7 @@
         <v>0.74800000000000111</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>0.48603351955306129</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1118,19 +1118,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E13">
         <f>C8-K8</f>
         <v>0.59575000000000244</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="O16">
         <f>AVERAGE(O4:O7)</f>
         <v>0.13080932749067697</v>
       </c>
     </row>
-    <row r="17" spans="15:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O17" t="s">
         <v>12</v>
       </c>
@@ -1148,18 +1148,18 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>0.91500000000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1222,7 +1222,7 @@
         <v>0.76000000000000512</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>0.96000000000000085</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>1.6600000000000037</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>2.1399999999999864</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1334,7 +1334,7 @@
       <c r="J8" s="5"/>
       <c r="O8" s="2"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1369,7 +1369,7 @@
       <c r="J9" s="5"/>
       <c r="O9" s="3"/>
     </row>
-    <row r="10" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1410,11 +1410,11 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -1531,12 +1531,12 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="12" max="12" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Fitted model and more measures
</commit_message>
<xml_diff>
--- a/Experimental Results/cell dry weight measurements.xlsx
+++ b/Experimental Results/cell dry weight measurements.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="135" windowWidth="14340" windowHeight="5835" activeTab="3"/>
+    <workbookView xWindow="396" yWindow="132" windowWidth="14340" windowHeight="5832" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Trial 1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="46">
   <si>
     <t xml:space="preserve">Date: </t>
   </si>
@@ -342,11 +342,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="44600320"/>
-        <c:axId val="44606208"/>
+        <c:axId val="130176512"/>
+        <c:axId val="130178048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="44600320"/>
+        <c:axId val="130176512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -356,12 +356,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44606208"/>
+        <c:crossAx val="130178048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="44606208"/>
+        <c:axId val="130178048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -372,7 +372,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44600320"/>
+        <c:crossAx val="130176512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -717,21 +717,21 @@
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -745,7 +745,7 @@
         <v>0.89500000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -786,7 +786,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -831,7 +831,7 @@
         <v>0.35999999999997812</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -880,7 +880,7 @@
         <v>0.50699999999999967</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -929,7 +929,7 @@
         <v>0.60299999999999976</v>
       </c>
     </row>
-    <row r="7" spans="1:16" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>4</v>
       </c>
@@ -978,7 +978,7 @@
         <v>0.74800000000000111</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>0.48603351955306129</v>
       </c>
     </row>
-    <row r="10" spans="1:16" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1118,19 +1118,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E13">
         <f>C8-K8</f>
         <v>0.59575000000000244</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="O16">
         <f>AVERAGE(O4:O7)</f>
         <v>0.13080932749067697</v>
       </c>
     </row>
-    <row r="17" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="15:15" ht="15" x14ac:dyDescent="0.25">
       <c r="O17" t="s">
         <v>12</v>
       </c>
@@ -1148,18 +1148,18 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>0.91500000000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="15" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1222,7 +1222,7 @@
         <v>0.76000000000000512</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="15" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>0.96000000000000085</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="15" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>1.6600000000000037</v>
       </c>
     </row>
-    <row r="7" spans="1:15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>2.1399999999999864</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1334,7 +1334,7 @@
       <c r="J8" s="5"/>
       <c r="O8" s="2"/>
     </row>
-    <row r="9" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1369,7 +1369,7 @@
       <c r="J9" s="5"/>
       <c r="O9" s="3"/>
     </row>
-    <row r="10" spans="1:15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1410,11 +1410,11 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -1528,15 +1528,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -1623,11 +1623,11 @@
         <v>0.63400000000000001</v>
       </c>
       <c r="L3">
-        <f>F15</f>
+        <f>G15</f>
         <v>0.4166666666666578</v>
       </c>
       <c r="M3">
-        <f>F16</f>
+        <f>G16</f>
         <v>2.8867513459484521E-2</v>
       </c>
     </row>
@@ -1782,13 +1782,16 @@
       <c r="C11" s="10">
         <v>42327</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="10">
+        <v>42331</v>
+      </c>
+      <c r="E11" t="s">
         <v>39</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>38</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1803,15 +1806,18 @@
         <v>2.8050000000000002</v>
       </c>
       <c r="D12">
+        <v>2.806</v>
+      </c>
+      <c r="E12">
         <f>C12-B12</f>
         <v>1.2000000000000011E-2</v>
       </c>
-      <c r="E12">
-        <f>D12-$G$3</f>
+      <c r="F12">
+        <f>E12-$G$3</f>
         <v>8.0000000000000071E-3</v>
       </c>
-      <c r="F12">
-        <f>E12/0.02</f>
+      <c r="G12">
+        <f>F12/0.02</f>
         <v>0.40000000000000036</v>
       </c>
     </row>
@@ -1826,15 +1832,18 @@
         <v>2.8</v>
       </c>
       <c r="D13">
-        <f t="shared" ref="D13:D14" si="3">C13-B13</f>
+        <v>2.8010000000000002</v>
+      </c>
+      <c r="E13">
+        <f>C13-B13</f>
         <v>1.2999999999999901E-2</v>
       </c>
-      <c r="E13">
-        <f t="shared" ref="E13:E14" si="4">D13-$G$3</f>
+      <c r="F13">
+        <f t="shared" ref="F13:F14" si="3">E13-$G$3</f>
         <v>8.999999999999897E-3</v>
       </c>
-      <c r="F13">
-        <f t="shared" ref="F13:F14" si="5">E13/0.02</f>
+      <c r="G13">
+        <f t="shared" ref="G13:G14" si="4">F13/0.02</f>
         <v>0.44999999999999485</v>
       </c>
     </row>
@@ -1849,15 +1858,18 @@
         <v>3.0019999999999998</v>
       </c>
       <c r="D14">
+        <v>3.0030000000000001</v>
+      </c>
+      <c r="E14">
+        <f>C14-B14</f>
+        <v>1.1999999999999567E-2</v>
+      </c>
+      <c r="F14">
         <f t="shared" si="3"/>
-        <v>1.1999999999999567E-2</v>
-      </c>
-      <c r="E14">
+        <v>7.999999999999563E-3</v>
+      </c>
+      <c r="G14">
         <f t="shared" si="4"/>
-        <v>7.999999999999563E-3</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="5"/>
         <v>0.39999999999997815</v>
       </c>
     </row>
@@ -1865,16 +1877,16 @@
       <c r="C15" t="s">
         <v>40</v>
       </c>
-      <c r="D15">
-        <f>AVERAGE(D12:D14)</f>
-        <v>1.233333333333316E-2</v>
-      </c>
       <c r="E15">
         <f>AVERAGE(E12:E14)</f>
-        <v>8.3333333333331563E-3</v>
+        <v>1.233333333333316E-2</v>
       </c>
       <c r="F15">
         <f>AVERAGE(F12:F14)</f>
+        <v>8.3333333333331563E-3</v>
+      </c>
+      <c r="G15">
+        <f>AVERAGE(G12:G14)</f>
         <v>0.4166666666666578</v>
       </c>
     </row>
@@ -1882,17 +1894,76 @@
       <c r="C16" t="s">
         <v>41</v>
       </c>
-      <c r="D16">
-        <f>STDEV(D12:D14)</f>
-        <v>5.7735026918969042E-4</v>
-      </c>
       <c r="E16">
         <f>STDEV(E12:E14)</f>
         <v>5.7735026918969042E-4</v>
       </c>
       <c r="F16">
         <f>STDEV(F12:F14)</f>
+        <v>5.7735026918969042E-4</v>
+      </c>
+      <c r="G16">
+        <f>STDEV(G12:G14)</f>
         <v>2.8867513459484521E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="10">
+        <v>42327</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="10">
+        <v>42331</v>
+      </c>
+      <c r="D18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>2.8159999999999998</v>
+      </c>
+      <c r="C19">
+        <v>2.831</v>
+      </c>
+      <c r="D19">
+        <f>C19-B19</f>
+        <v>1.5000000000000124E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20">
+        <v>3.2570000000000001</v>
+      </c>
+      <c r="C20">
+        <v>3.2709999999999999</v>
+      </c>
+      <c r="D20">
+        <f t="shared" ref="D20:D21" si="5">C20-B20</f>
+        <v>1.399999999999979E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21">
+        <v>3.3109999999999999</v>
+      </c>
+      <c r="C21">
+        <v>3.3210000000000002</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="5"/>
+        <v>1.0000000000000231E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nov update and figs
</commit_message>
<xml_diff>
--- a/Experimental Results/cell dry weight measurements.xlsx
+++ b/Experimental Results/cell dry weight measurements.xlsx
@@ -342,11 +342,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="44600320"/>
-        <c:axId val="44606208"/>
+        <c:axId val="55669504"/>
+        <c:axId val="55671040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="44600320"/>
+        <c:axId val="55669504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -356,12 +356,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44606208"/>
+        <c:crossAx val="55671040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="44606208"/>
+        <c:axId val="55671040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -372,7 +372,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44600320"/>
+        <c:crossAx val="55669504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -394,15 +394,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>200810</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>125281</xdr:rowOff>
+      <xdr:colOff>155986</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>147693</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>505610</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>125281</xdr:rowOff>
+      <xdr:colOff>460786</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>147693</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1530,8 +1530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
More dilution and DCW data
</commit_message>
<xml_diff>
--- a/Experimental Results/cell dry weight measurements.xlsx
+++ b/Experimental Results/cell dry weight measurements.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="396" yWindow="132" windowWidth="14340" windowHeight="5832" activeTab="3"/>
+    <workbookView xWindow="396" yWindow="132" windowWidth="14340" windowHeight="5832" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Trial 1" sheetId="1" r:id="rId1"/>
     <sheet name="Trial 2" sheetId="2" r:id="rId2"/>
     <sheet name="Salts Calculations" sheetId="3" r:id="rId3"/>
     <sheet name="Filtering Method" sheetId="4" r:id="rId4"/>
+    <sheet name="Filtering and Spin" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="70">
   <si>
     <t xml:space="preserve">Date: </t>
   </si>
@@ -191,13 +192,49 @@
   </si>
   <si>
     <t>Predict Y</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>End Wt (g)</t>
+  </si>
+  <si>
+    <t>Start Wt (g)</t>
+  </si>
+  <si>
+    <t>Control Adjust</t>
+  </si>
+  <si>
+    <t>Final Wt (g)</t>
+  </si>
+  <si>
+    <t>Control 1</t>
+  </si>
+  <si>
+    <t>Control 2</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Average Ctrl.</t>
+  </si>
+  <si>
+    <t>Ctrl. Stdev.</t>
+  </si>
+  <si>
+    <t>Final Density (g/L)</t>
+  </si>
+  <si>
+    <t>Local Density (g/L)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,8 +242,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -216,6 +261,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -269,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -281,6 +332,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,11 +459,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="137385472"/>
-        <c:axId val="137387008"/>
+        <c:axId val="131544960"/>
+        <c:axId val="131546496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="137385472"/>
+        <c:axId val="131544960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -416,12 +473,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137387008"/>
+        <c:crossAx val="131546496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="137387008"/>
+        <c:axId val="131546496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -432,7 +489,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137385472"/>
+        <c:crossAx val="131544960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -479,7 +536,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -604,11 +660,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="137407872"/>
-        <c:axId val="137565696"/>
+        <c:axId val="131575808"/>
+        <c:axId val="131577728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="137407872"/>
+        <c:axId val="131575808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -630,19 +686,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137565696"/>
+        <c:crossAx val="131577728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="137565696"/>
+        <c:axId val="131577728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -665,18 +720,156 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137407872"/>
+        <c:crossAx val="131575808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:intercept val="0"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.3675726159230096"/>
+                  <c:y val="-0.20096821230679499"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Filtering and Spin'!$C$8:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.63400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.63400000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Filtering and Spin'!$H$8:$H$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.30999999999998806</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.30999999999998806</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="81296384"/>
+        <c:axId val="81293312"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="81296384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="81293312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="81293312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="81296384"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -746,6 +939,41 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>17930</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>49306</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>484094</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>103095</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2013,7 +2241,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
@@ -2712,4 +2940,404 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="11">
+        <v>42341</v>
+      </c>
+      <c r="B2" s="12">
+        <v>1</v>
+      </c>
+      <c r="C2" s="12">
+        <v>0.63</v>
+      </c>
+      <c r="D2" s="12">
+        <v>3.0960000000000001</v>
+      </c>
+      <c r="E2" s="12">
+        <v>3.1190000000000002</v>
+      </c>
+      <c r="F2" s="12">
+        <f>E2-$F$7</f>
+        <v>3.1115000000000004</v>
+      </c>
+      <c r="G2" s="12">
+        <f>F2-D2</f>
+        <v>1.5500000000000291E-2</v>
+      </c>
+      <c r="H2" s="12">
+        <f>G2/0.05</f>
+        <v>0.31000000000000583</v>
+      </c>
+      <c r="I2" s="12">
+        <f>H2/C2</f>
+        <v>0.49206349206350131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="11">
+        <v>42341</v>
+      </c>
+      <c r="B3" s="12">
+        <v>2</v>
+      </c>
+      <c r="C3" s="12">
+        <v>0.63</v>
+      </c>
+      <c r="D3" s="12">
+        <v>2.5110000000000001</v>
+      </c>
+      <c r="E3" s="12">
+        <v>2.5329999999999999</v>
+      </c>
+      <c r="F3" s="12">
+        <f t="shared" ref="F3:F5" si="0">E3-$F$7</f>
+        <v>2.5255000000000001</v>
+      </c>
+      <c r="G3" s="12">
+        <f t="shared" ref="G3:G5" si="1">F3-D3</f>
+        <v>1.4499999999999957E-2</v>
+      </c>
+      <c r="H3" s="12">
+        <f t="shared" ref="H3:H11" si="2">G3/0.05</f>
+        <v>0.28999999999999915</v>
+      </c>
+      <c r="I3" s="12">
+        <f t="shared" ref="I3:I5" si="3">H3/C3</f>
+        <v>0.46031746031745896</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="10">
+        <v>42341</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>0.626</v>
+      </c>
+      <c r="D4">
+        <v>2.5659999999999998</v>
+      </c>
+      <c r="E4">
+        <v>2.593</v>
+      </c>
+      <c r="F4" s="13">
+        <f t="shared" si="0"/>
+        <v>2.5854999999999997</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>1.9499999999999851E-2</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="2"/>
+        <v>0.38999999999999702</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="3"/>
+        <v>0.62300319488817413</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="11">
+        <v>42341</v>
+      </c>
+      <c r="B5" s="12">
+        <v>4</v>
+      </c>
+      <c r="C5" s="12">
+        <v>0.626</v>
+      </c>
+      <c r="D5" s="12">
+        <v>2.673</v>
+      </c>
+      <c r="E5" s="12">
+        <v>2.6930000000000001</v>
+      </c>
+      <c r="F5" s="12">
+        <f t="shared" si="0"/>
+        <v>2.6855000000000002</v>
+      </c>
+      <c r="G5" s="12">
+        <f t="shared" si="1"/>
+        <v>1.2500000000000178E-2</v>
+      </c>
+      <c r="H5" s="12">
+        <f t="shared" si="2"/>
+        <v>0.25000000000000355</v>
+      </c>
+      <c r="I5" s="12">
+        <f t="shared" si="3"/>
+        <v>0.39936102236422294</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="14">
+        <v>42342</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="13">
+        <v>2.88</v>
+      </c>
+      <c r="E6" s="13">
+        <v>2.887</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+    </row>
+    <row r="7" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="14">
+        <v>42342</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="13">
+        <v>2.6019999999999999</v>
+      </c>
+      <c r="E7" s="13">
+        <v>2.61</v>
+      </c>
+      <c r="F7" s="13">
+        <f>AVERAGE((E6-D6),(E7-D7))</f>
+        <v>7.5000000000000622E-3</v>
+      </c>
+      <c r="G7" s="13">
+        <f>STDEV((E6-D6),(E7-D7))</f>
+        <v>7.0710678118646967E-4</v>
+      </c>
+      <c r="H7" s="16"/>
+      <c r="I7" s="15"/>
+    </row>
+    <row r="8" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="14">
+        <v>42343</v>
+      </c>
+      <c r="B8" s="13">
+        <v>1</v>
+      </c>
+      <c r="C8" s="13">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="D8" s="13">
+        <v>2.8330000000000002</v>
+      </c>
+      <c r="E8" s="13">
+        <v>2.8559999999999999</v>
+      </c>
+      <c r="F8" s="13">
+        <f t="shared" ref="F8:F11" si="4">E8-$F$7</f>
+        <v>2.8484999999999996</v>
+      </c>
+      <c r="G8">
+        <f t="shared" ref="G8:G11" si="5">F8-D8</f>
+        <v>1.5499999999999403E-2</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="2"/>
+        <v>0.30999999999998806</v>
+      </c>
+      <c r="I8">
+        <f>H8/C8</f>
+        <v>0.48895899053625874</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="14">
+        <v>42343</v>
+      </c>
+      <c r="B9" s="13">
+        <v>2</v>
+      </c>
+      <c r="C9" s="13">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="D9" s="13">
+        <v>2.8620000000000001</v>
+      </c>
+      <c r="E9" s="13">
+        <v>2.8849999999999998</v>
+      </c>
+      <c r="F9" s="13">
+        <f t="shared" si="4"/>
+        <v>2.8774999999999995</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="5"/>
+        <v>1.5499999999999403E-2</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="2"/>
+        <v>0.30999999999998806</v>
+      </c>
+      <c r="I9">
+        <f t="shared" ref="I9:I11" si="6">H9/C9</f>
+        <v>0.48895899053625874</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="14">
+        <v>42345</v>
+      </c>
+      <c r="B10" s="13">
+        <v>1</v>
+      </c>
+      <c r="C10" s="13">
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="D10" s="13">
+        <v>3.0019999999999998</v>
+      </c>
+      <c r="E10" s="13">
+        <v>3.028</v>
+      </c>
+      <c r="F10" s="13">
+        <f t="shared" si="4"/>
+        <v>3.0205000000000002</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="5"/>
+        <v>1.8500000000000405E-2</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>0.3700000000000081</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="6"/>
+        <v>0.55891238670696086</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="14">
+        <v>42345</v>
+      </c>
+      <c r="B11" s="13">
+        <v>2</v>
+      </c>
+      <c r="C11" s="13">
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="D11" s="13">
+        <v>3.1480000000000001</v>
+      </c>
+      <c r="E11" s="13">
+        <v>3.173</v>
+      </c>
+      <c r="F11" s="13">
+        <f t="shared" si="4"/>
+        <v>3.1654999999999998</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="5"/>
+        <v>1.7499999999999627E-2</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="2"/>
+        <v>0.34999999999999254</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="6"/>
+        <v>0.52870090634439959</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="10">
+        <v>42346</v>
+      </c>
+      <c r="B12" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="10">
+        <v>42346</v>
+      </c>
+      <c r="B13" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="10">
+        <v>42347</v>
+      </c>
+      <c r="B14" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="10">
+        <v>42347</v>
+      </c>
+      <c r="B15" s="13">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
LOOCV and other things
</commit_message>
<xml_diff>
--- a/Experimental Results/cell dry weight measurements.xlsx
+++ b/Experimental Results/cell dry weight measurements.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="396" yWindow="132" windowWidth="14340" windowHeight="5832" activeTab="4"/>
+    <workbookView xWindow="390" yWindow="135" windowWidth="14340" windowHeight="5835" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Trial 1" sheetId="1" r:id="rId1"/>
@@ -459,11 +459,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="131544960"/>
-        <c:axId val="131546496"/>
+        <c:axId val="79001472"/>
+        <c:axId val="79003008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="131544960"/>
+        <c:axId val="79001472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -473,12 +473,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131546496"/>
+        <c:crossAx val="79003008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="131546496"/>
+        <c:axId val="79003008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -489,7 +489,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131544960"/>
+        <c:crossAx val="79001472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -660,11 +660,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="131575808"/>
-        <c:axId val="131577728"/>
+        <c:axId val="41211392"/>
+        <c:axId val="41213312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="131575808"/>
+        <c:axId val="41211392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -692,12 +692,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131577728"/>
+        <c:crossAx val="41213312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="131577728"/>
+        <c:axId val="41213312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -726,7 +726,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131575808"/>
+        <c:crossAx val="41211392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -779,8 +779,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.3675726159230096"/>
-                  <c:y val="-0.20096821230679499"/>
+                  <c:x val="-0.43199805248818512"/>
+                  <c:y val="7.6497730043290108E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -826,11 +826,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="81296384"/>
-        <c:axId val="81293312"/>
+        <c:axId val="42777600"/>
+        <c:axId val="52495104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81296384"/>
+        <c:axId val="42777600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -840,12 +840,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81293312"/>
+        <c:crossAx val="52495104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81293312"/>
+        <c:axId val="52495104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -856,20 +856,11 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81296384"/>
+        <c:crossAx val="42777600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:legendEntry>
-        <c:idx val="1"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -951,16 +942,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>17930</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>49306</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>286871</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>94130</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>484094</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>103095</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>338418</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>147919</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1275,21 +1266,21 @@
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1303,7 +1294,7 @@
         <v>0.89500000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1344,7 +1335,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1389,7 +1380,7 @@
         <v>0.35999999999997812</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1438,7 +1429,7 @@
         <v>0.50699999999999967</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1487,7 +1478,7 @@
         <v>0.60299999999999976</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1536,7 +1527,7 @@
         <v>0.74800000000000111</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1584,7 +1575,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1634,7 +1625,7 @@
         <v>0.48603351955306129</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1676,19 +1667,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E13">
         <f>C8-K8</f>
         <v>0.59575000000000244</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="O16">
         <f>AVERAGE(O4:O7)</f>
         <v>0.13080932749067697</v>
       </c>
     </row>
-    <row r="17" spans="15:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O17" t="s">
         <v>12</v>
       </c>
@@ -1706,18 +1697,18 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1731,7 +1722,7 @@
         <v>0.91500000000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1772,7 +1763,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1818,7 +1809,7 @@
         <v>0.76000000000000512</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1868,7 +1859,7 @@
         <v>0.96799999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1918,7 +1909,7 @@
         <v>2.0679999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1968,7 +1959,7 @@
         <v>2.8359999999999985</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -2016,7 +2007,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -2066,7 +2057,7 @@
         <v>1.5081967213114742</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -2121,11 +2112,11 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -2245,12 +2236,12 @@
       <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="12" max="12" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="10">
         <v>42320</v>
       </c>
@@ -2273,7 +2264,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -2313,7 +2304,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -2360,7 +2351,7 @@
         <v>0.60000000000000053</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2409,7 +2400,7 @@
         <v>0.54999999999998384</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -2447,7 +2438,7 @@
         <v>0.50000000000001155</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -2485,7 +2476,7 @@
         <v>0.44999999999999485</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="F7" t="s">
         <v>40</v>
       </c>
@@ -2508,7 +2499,7 @@
         <v>0.50000000000001155</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="F8" t="s">
         <v>41</v>
       </c>
@@ -2531,7 +2522,7 @@
         <v>0.34999999999998366</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="O9">
         <v>0.69199999999999995</v>
       </c>
@@ -2539,7 +2530,7 @@
         <v>0.45000000000001705</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="10">
         <v>42326</v>
       </c>
@@ -2556,7 +2547,7 @@
         <v>0.44999999999999485</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -2588,7 +2579,7 @@
         <v>0.30000000000001137</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -2617,7 +2608,7 @@
         <v>0.44999999999999485</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2646,7 +2637,7 @@
         <v>0.50000000000001155</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>3</v>
       </c>
@@ -2675,7 +2666,7 @@
         <v>0.34999999999998366</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>40</v>
       </c>
@@ -2692,7 +2683,7 @@
         <v>0.43333333333333002</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>41</v>
       </c>
@@ -2709,7 +2700,7 @@
         <v>7.6376261582610933E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:29" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
         <v>42327</v>
       </c>
@@ -2720,7 +2711,7 @@
         <v>0.69199999999999995</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:29" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>36</v>
       </c>
@@ -2740,7 +2731,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -2766,7 +2757,7 @@
         <v>0.45000000000001705</v>
       </c>
     </row>
-    <row r="21" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2</v>
       </c>
@@ -2792,7 +2783,7 @@
         <v>0.44999999999999485</v>
       </c>
     </row>
-    <row r="22" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>3</v>
       </c>
@@ -2836,7 +2827,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
         <v>46</v>
       </c>
@@ -2873,7 +2864,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
         <v>42</v>
       </c>
@@ -2910,7 +2901,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="25" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="W25" t="s">
         <v>55</v>
       </c>
@@ -2947,16 +2938,16 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -3251,24 +3242,21 @@
       <c r="D10" s="13">
         <v>3.0019999999999998</v>
       </c>
-      <c r="E10" s="13">
-        <v>3.028</v>
-      </c>
       <c r="F10" s="13">
         <f t="shared" si="4"/>
-        <v>3.0205000000000002</v>
+        <v>-7.5000000000000622E-3</v>
       </c>
       <c r="G10">
         <f t="shared" si="5"/>
-        <v>1.8500000000000405E-2</v>
+        <v>-3.0095000000000001</v>
       </c>
       <c r="H10">
         <f t="shared" si="2"/>
-        <v>0.3700000000000081</v>
+        <v>-60.19</v>
       </c>
       <c r="I10">
         <f t="shared" si="6"/>
-        <v>0.55891238670696086</v>
+        <v>-90.9214501510574</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
@@ -3284,24 +3272,21 @@
       <c r="D11" s="13">
         <v>3.1480000000000001</v>
       </c>
-      <c r="E11" s="13">
-        <v>3.173</v>
-      </c>
       <c r="F11" s="13">
         <f t="shared" si="4"/>
-        <v>3.1654999999999998</v>
+        <v>-7.5000000000000622E-3</v>
       </c>
       <c r="G11">
         <f t="shared" si="5"/>
-        <v>1.7499999999999627E-2</v>
+        <v>-3.1555</v>
       </c>
       <c r="H11">
         <f t="shared" si="2"/>
-        <v>0.34999999999999254</v>
+        <v>-63.11</v>
       </c>
       <c r="I11">
         <f t="shared" si="6"/>
-        <v>0.52870090634439959</v>
+        <v>-95.332326283987911</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
More wet lab points
</commit_message>
<xml_diff>
--- a/Experimental Results/cell dry weight measurements.xlsx
+++ b/Experimental Results/cell dry weight measurements.xlsx
@@ -411,10 +411,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Filtering and Spin'!$C$10:$C$18</c:f>
+              <c:f>'Filtering and Spin'!$C$10:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.63400000000000001</c:v>
                 </c:pt>
@@ -441,16 +441,22 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.78600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.46600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.46600000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Filtering and Spin'!$H$10:$H$18</c:f>
+              <c:f>'Filtering and Spin'!$H$10:$H$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.26999999999999247</c:v>
                 </c:pt>
@@ -473,10 +479,16 @@
                   <c:v>0.38999999999999702</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.43000000000000149</c:v>
+                  <c:v>0.38999999999999702</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.34999999999999254</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1699999999999946</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.1899999999999924</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -491,11 +503,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="135849856"/>
-        <c:axId val="135851392"/>
+        <c:axId val="146139008"/>
+        <c:axId val="146140544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="135849856"/>
+        <c:axId val="146139008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -515,12 +527,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="135851392"/>
+        <c:crossAx val="146140544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="135851392"/>
+        <c:axId val="146140544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -541,7 +553,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="135849856"/>
+        <c:crossAx val="146139008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -660,11 +672,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="136749056"/>
-        <c:axId val="136750592"/>
+        <c:axId val="146780160"/>
+        <c:axId val="146781696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="136749056"/>
+        <c:axId val="146780160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -674,12 +686,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136750592"/>
+        <c:crossAx val="146781696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="136750592"/>
+        <c:axId val="146781696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -690,7 +702,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136749056"/>
+        <c:crossAx val="146780160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -861,11 +873,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="137914240"/>
-        <c:axId val="137916416"/>
+        <c:axId val="147154816"/>
+        <c:axId val="147156992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="137914240"/>
+        <c:axId val="147154816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -893,12 +905,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137916416"/>
+        <c:crossAx val="147156992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="137916416"/>
+        <c:axId val="147156992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -927,7 +939,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137914240"/>
+        <c:crossAx val="147154816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1334,10 +1346,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1436,7 +1448,7 @@
         <v>1.3499999999999623E-2</v>
       </c>
       <c r="H3" s="12">
-        <f t="shared" ref="H3:H18" si="2">G3/0.05</f>
+        <f t="shared" ref="H3:H20" si="2">G3/0.05</f>
         <v>0.26999999999999247</v>
       </c>
       <c r="I3" s="12">
@@ -1620,11 +1632,11 @@
         <v>2.855</v>
       </c>
       <c r="F10" s="13">
-        <f t="shared" ref="F10:F18" si="4">E10-$F$8</f>
+        <f t="shared" ref="F10:F20" si="4">E10-$F$8</f>
         <v>2.8464999999999998</v>
       </c>
       <c r="G10">
-        <f t="shared" ref="G10:G18" si="5">F10-D10</f>
+        <f t="shared" ref="G10:G20" si="5">F10-D10</f>
         <v>1.3499999999999623E-2</v>
       </c>
       <c r="H10">
@@ -1665,7 +1677,7 @@
         <v>0.26999999999999247</v>
       </c>
       <c r="I11">
-        <f t="shared" ref="I11:I18" si="6">H11/C11</f>
+        <f t="shared" ref="I11:I20" si="6">H11/C11</f>
         <v>0.42586750788642347</v>
       </c>
     </row>
@@ -1848,23 +1860,23 @@
         <v>2.835</v>
       </c>
       <c r="E17" s="13">
-        <v>2.8650000000000002</v>
+        <v>2.863</v>
       </c>
       <c r="F17" s="13">
         <f t="shared" si="4"/>
-        <v>2.8565</v>
+        <v>2.8544999999999998</v>
       </c>
       <c r="G17">
         <f t="shared" si="5"/>
-        <v>2.1500000000000075E-2</v>
+        <v>1.9499999999999851E-2</v>
       </c>
       <c r="H17">
         <f t="shared" si="2"/>
-        <v>0.43000000000000149</v>
+        <v>0.38999999999999702</v>
       </c>
       <c r="I17">
         <f t="shared" si="6"/>
-        <v>0.54707379134860235</v>
+        <v>0.49618320610686639</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -1913,6 +1925,25 @@
       <c r="D19" s="13">
         <v>3.08</v>
       </c>
+      <c r="E19" s="13">
+        <v>3.097</v>
+      </c>
+      <c r="F19" s="13">
+        <f t="shared" si="4"/>
+        <v>3.0884999999999998</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="5"/>
+        <v>8.49999999999973E-3</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="2"/>
+        <v>0.1699999999999946</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="6"/>
+        <v>0.36480686695277809</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="10">
@@ -1926,6 +1957,53 @@
       </c>
       <c r="D20" s="13">
         <v>2.859</v>
+      </c>
+      <c r="E20" s="13">
+        <v>2.8769999999999998</v>
+      </c>
+      <c r="F20" s="13">
+        <f t="shared" si="4"/>
+        <v>2.8684999999999996</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="5"/>
+        <v>9.4999999999996199E-3</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="2"/>
+        <v>0.1899999999999924</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="6"/>
+        <v>0.40772532188839566</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="10">
+        <v>42355</v>
+      </c>
+      <c r="B21" s="13">
+        <v>1</v>
+      </c>
+      <c r="C21" s="13">
+        <v>0.88</v>
+      </c>
+      <c r="D21" s="13">
+        <v>2.5099999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="10">
+        <v>42355</v>
+      </c>
+      <c r="B22" s="13">
+        <v>2</v>
+      </c>
+      <c r="C22" s="13">
+        <v>0.88</v>
+      </c>
+      <c r="D22" s="13">
+        <v>2.7559999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More OD DCW data
</commit_message>
<xml_diff>
--- a/Experimental Results/cell dry weight measurements.xlsx
+++ b/Experimental Results/cell dry weight measurements.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="396" yWindow="132" windowWidth="14340" windowHeight="5832" activeTab="1"/>
+    <workbookView xWindow="396" yWindow="132" windowWidth="14340" windowHeight="5832"/>
   </bookViews>
   <sheets>
     <sheet name="Filtering and Spin" sheetId="5" r:id="rId1"/>
@@ -411,10 +411,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Filtering and Spin'!$C$10:$C$20</c:f>
+              <c:f>'Filtering and Spin'!$C$10:$C$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>0.63400000000000001</c:v>
                 </c:pt>
@@ -447,16 +447,22 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.46600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.88</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.88</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Filtering and Spin'!$H$10:$H$20</c:f>
+              <c:f>'Filtering and Spin'!$H$10:$H$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>0.26999999999999247</c:v>
                 </c:pt>
@@ -482,13 +488,19 @@
                   <c:v>0.38999999999999702</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.34999999999999254</c:v>
+                  <c:v>0.36999999999999922</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.1699999999999946</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.1899999999999924</c:v>
+                  <c:v>0.1699999999999946</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.44999999999999929</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.43000000000000149</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -503,11 +515,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="146139008"/>
-        <c:axId val="146140544"/>
+        <c:axId val="127133568"/>
+        <c:axId val="127135104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="146139008"/>
+        <c:axId val="127133568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -527,12 +539,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146140544"/>
+        <c:crossAx val="127135104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="146140544"/>
+        <c:axId val="127135104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -553,7 +565,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146139008"/>
+        <c:crossAx val="127133568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -672,11 +684,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="146780160"/>
-        <c:axId val="146781696"/>
+        <c:axId val="131969024"/>
+        <c:axId val="131970560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="146780160"/>
+        <c:axId val="131969024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -686,12 +698,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146781696"/>
+        <c:crossAx val="131970560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="146781696"/>
+        <c:axId val="131970560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -702,7 +714,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146780160"/>
+        <c:crossAx val="131969024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -873,11 +885,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="147154816"/>
-        <c:axId val="147156992"/>
+        <c:axId val="134571904"/>
+        <c:axId val="134574080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="147154816"/>
+        <c:axId val="134571904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -905,12 +917,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147156992"/>
+        <c:crossAx val="134574080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="147156992"/>
+        <c:axId val="134574080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -939,7 +951,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147154816"/>
+        <c:crossAx val="134571904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -960,7 +972,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="60" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1348,8 +1360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1448,7 +1460,7 @@
         <v>1.3499999999999623E-2</v>
       </c>
       <c r="H3" s="12">
-        <f t="shared" ref="H3:H20" si="2">G3/0.05</f>
+        <f t="shared" ref="H3:H22" si="2">G3/0.05</f>
         <v>0.26999999999999247</v>
       </c>
       <c r="I3" s="12">
@@ -1632,11 +1644,11 @@
         <v>2.855</v>
       </c>
       <c r="F10" s="13">
-        <f t="shared" ref="F10:F20" si="4">E10-$F$8</f>
+        <f t="shared" ref="F10:F22" si="4">E10-$F$8</f>
         <v>2.8464999999999998</v>
       </c>
       <c r="G10">
-        <f t="shared" ref="G10:G20" si="5">F10-D10</f>
+        <f t="shared" ref="G10:G22" si="5">F10-D10</f>
         <v>1.3499999999999623E-2</v>
       </c>
       <c r="H10">
@@ -1677,7 +1689,7 @@
         <v>0.26999999999999247</v>
       </c>
       <c r="I11">
-        <f t="shared" ref="I11:I20" si="6">H11/C11</f>
+        <f t="shared" ref="I11:I22" si="6">H11/C11</f>
         <v>0.42586750788642347</v>
       </c>
     </row>
@@ -1893,23 +1905,23 @@
         <v>2.871</v>
       </c>
       <c r="E18" s="13">
-        <v>2.8969999999999998</v>
+        <v>2.8980000000000001</v>
       </c>
       <c r="F18" s="13">
         <f t="shared" si="4"/>
-        <v>2.8884999999999996</v>
+        <v>2.8895</v>
       </c>
       <c r="G18">
         <f t="shared" si="5"/>
-        <v>1.7499999999999627E-2</v>
+        <v>1.8499999999999961E-2</v>
       </c>
       <c r="H18">
         <f t="shared" si="2"/>
-        <v>0.34999999999999254</v>
+        <v>0.36999999999999922</v>
       </c>
       <c r="I18">
         <f t="shared" si="6"/>
-        <v>0.44529262086513044</v>
+        <v>0.47073791348600408</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -1959,23 +1971,23 @@
         <v>2.859</v>
       </c>
       <c r="E20" s="13">
-        <v>2.8769999999999998</v>
+        <v>2.8759999999999999</v>
       </c>
       <c r="F20" s="13">
         <f t="shared" si="4"/>
-        <v>2.8684999999999996</v>
+        <v>2.8674999999999997</v>
       </c>
       <c r="G20">
         <f t="shared" si="5"/>
-        <v>9.4999999999996199E-3</v>
+        <v>8.49999999999973E-3</v>
       </c>
       <c r="H20">
         <f t="shared" si="2"/>
-        <v>0.1899999999999924</v>
+        <v>0.1699999999999946</v>
       </c>
       <c r="I20">
         <f t="shared" si="6"/>
-        <v>0.40772532188839566</v>
+        <v>0.36480686695277809</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -1991,6 +2003,25 @@
       <c r="D21" s="13">
         <v>2.5099999999999998</v>
       </c>
+      <c r="E21" s="13">
+        <v>2.5409999999999999</v>
+      </c>
+      <c r="F21" s="13">
+        <f t="shared" si="4"/>
+        <v>2.5324999999999998</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="5"/>
+        <v>2.2499999999999964E-2</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="2"/>
+        <v>0.44999999999999929</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="6"/>
+        <v>0.51136363636363558</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="10">
@@ -2004,6 +2035,25 @@
       </c>
       <c r="D22" s="13">
         <v>2.7559999999999998</v>
+      </c>
+      <c r="E22" s="13">
+        <v>2.786</v>
+      </c>
+      <c r="F22" s="13">
+        <f t="shared" si="4"/>
+        <v>2.7774999999999999</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="5"/>
+        <v>2.1500000000000075E-2</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="2"/>
+        <v>0.43000000000000149</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="6"/>
+        <v>0.48863636363636531</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New GC and OD_DCW Numbers
</commit_message>
<xml_diff>
--- a/Experimental Results/cell dry weight measurements.xlsx
+++ b/Experimental Results/cell dry weight measurements.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="135" windowWidth="14340" windowHeight="5835" activeTab="1"/>
+    <workbookView xWindow="396" yWindow="132" windowWidth="14340" windowHeight="5832"/>
   </bookViews>
   <sheets>
     <sheet name="Filtering and Spin" sheetId="5" r:id="rId1"/>
@@ -488,16 +488,16 @@
                   <c:v>0.38999999999999702</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.36999999999999922</c:v>
+                  <c:v>0.32999999999999474</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.1699999999999946</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.1699999999999946</c:v>
+                  <c:v>0.1499999999999968</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.44999999999999929</c:v>
+                  <c:v>0.43000000000000149</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0.43000000000000149</c:v>
@@ -515,11 +515,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="106329984"/>
-        <c:axId val="106331520"/>
+        <c:axId val="137029504"/>
+        <c:axId val="137031040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="106329984"/>
+        <c:axId val="137029504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -539,12 +539,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="106331520"/>
+        <c:crossAx val="137031040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="106331520"/>
+        <c:axId val="137031040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -565,7 +565,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="106329984"/>
+        <c:crossAx val="137029504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -684,11 +684,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="113926144"/>
-        <c:axId val="113927680"/>
+        <c:axId val="148160512"/>
+        <c:axId val="148162048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="113926144"/>
+        <c:axId val="148160512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -698,12 +698,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113927680"/>
+        <c:crossAx val="148162048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="113927680"/>
+        <c:axId val="148162048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -714,7 +714,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113926144"/>
+        <c:crossAx val="148160512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -885,11 +885,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="113952640"/>
-        <c:axId val="113958912"/>
+        <c:axId val="148531072"/>
+        <c:axId val="148533248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="113952640"/>
+        <c:axId val="148531072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -917,12 +917,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113958912"/>
+        <c:crossAx val="148533248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="113958912"/>
+        <c:axId val="148533248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -951,7 +951,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113952640"/>
+        <c:crossAx val="148531072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -972,7 +972,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="60" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -983,7 +983,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8670000" cy="6300000"/>
+    <xdr:ext cx="8661400" cy="6286500"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -1358,22 +1358,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -1402,7 +1402,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="11">
         <v>42341</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>0.46031746031745896</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <v>42341</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>1.3499999999999623E-2</v>
       </c>
       <c r="H3" s="12">
-        <f t="shared" ref="H3:H22" si="2">G3/0.05</f>
+        <f t="shared" ref="H3:H24" si="2">G3/0.05</f>
         <v>0.26999999999999247</v>
       </c>
       <c r="I3" s="12">
@@ -1468,7 +1468,7 @@
         <v>0.42857142857141661</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="10">
         <v>42341</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>0.59105431309904033</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="11">
         <v>42341</v>
       </c>
@@ -1534,7 +1534,7 @@
         <v>0.36741214057507487</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>42349</v>
       </c>
@@ -1570,7 +1570,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="13" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14">
         <v>42342</v>
       </c>
@@ -1595,7 +1595,7 @@
       <c r="H7" s="15"/>
       <c r="I7" s="15"/>
     </row>
-    <row r="8" spans="1:10" s="13" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14">
         <v>42342</v>
       </c>
@@ -1622,12 +1622,12 @@
       <c r="H8" s="16"/>
       <c r="I8" s="15"/>
     </row>
-    <row r="9" spans="1:10" s="13" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="H9" s="16"/>
       <c r="I9" s="15"/>
     </row>
-    <row r="10" spans="1:10" s="13" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14">
         <v>42343</v>
       </c>
@@ -1644,11 +1644,11 @@
         <v>2.855</v>
       </c>
       <c r="F10" s="13">
-        <f t="shared" ref="F10:F22" si="4">E10-$F$8</f>
+        <f t="shared" ref="F10:F24" si="4">E10-$F$8</f>
         <v>2.8464999999999998</v>
       </c>
       <c r="G10">
-        <f t="shared" ref="G10:G22" si="5">F10-D10</f>
+        <f t="shared" ref="G10:G24" si="5">F10-D10</f>
         <v>1.3499999999999623E-2</v>
       </c>
       <c r="H10">
@@ -1660,7 +1660,7 @@
         <v>0.42586750788642347</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="13" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14">
         <v>42343</v>
       </c>
@@ -1689,11 +1689,11 @@
         <v>0.26999999999999247</v>
       </c>
       <c r="I11">
-        <f t="shared" ref="I11:I22" si="6">H11/C11</f>
+        <f t="shared" ref="I11:I24" si="6">H11/C11</f>
         <v>0.42586750788642347</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="13" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="14">
         <v>42345</v>
       </c>
@@ -1726,7 +1726,7 @@
         <v>0.49848942598187856</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="13" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="14">
         <v>42345</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>0.37764350453171397</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="10">
         <v>42346</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>0.60355029585799003</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
         <v>42346</v>
       </c>
@@ -1825,7 +1825,7 @@
         <v>0.43786982248519568</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="10">
         <v>42349</v>
       </c>
@@ -1858,7 +1858,7 @@
         <v>0.45882352941176119</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
         <v>42353</v>
       </c>
@@ -1891,7 +1891,7 @@
         <v>0.49618320610686639</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
         <v>42353</v>
       </c>
@@ -1905,26 +1905,26 @@
         <v>2.871</v>
       </c>
       <c r="E18" s="13">
-        <v>2.8980000000000001</v>
+        <v>2.8959999999999999</v>
       </c>
       <c r="F18" s="13">
         <f t="shared" si="4"/>
-        <v>2.8895</v>
+        <v>2.8874999999999997</v>
       </c>
       <c r="G18">
         <f t="shared" si="5"/>
-        <v>1.8499999999999961E-2</v>
+        <v>1.6499999999999737E-2</v>
       </c>
       <c r="H18">
         <f t="shared" si="2"/>
-        <v>0.36999999999999922</v>
+        <v>0.32999999999999474</v>
       </c>
       <c r="I18">
         <f t="shared" si="6"/>
-        <v>0.47073791348600408</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+        <v>0.41984732824426813</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="10">
         <v>42354</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>0.36480686695277809</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="10">
         <v>42354</v>
       </c>
@@ -1971,26 +1971,26 @@
         <v>2.859</v>
       </c>
       <c r="E20" s="13">
-        <v>2.8759999999999999</v>
+        <v>2.875</v>
       </c>
       <c r="F20" s="13">
         <f t="shared" si="4"/>
-        <v>2.8674999999999997</v>
+        <v>2.8664999999999998</v>
       </c>
       <c r="G20">
         <f t="shared" si="5"/>
-        <v>8.49999999999973E-3</v>
+        <v>7.4999999999998401E-3</v>
       </c>
       <c r="H20">
         <f t="shared" si="2"/>
-        <v>0.1699999999999946</v>
+        <v>0.1499999999999968</v>
       </c>
       <c r="I20">
         <f t="shared" si="6"/>
-        <v>0.36480686695277809</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+        <v>0.32188841201716051</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="10">
         <v>42355</v>
       </c>
@@ -2004,26 +2004,26 @@
         <v>2.5099999999999998</v>
       </c>
       <c r="E21" s="13">
-        <v>2.5409999999999999</v>
+        <v>2.54</v>
       </c>
       <c r="F21" s="13">
         <f t="shared" si="4"/>
-        <v>2.5324999999999998</v>
+        <v>2.5314999999999999</v>
       </c>
       <c r="G21">
         <f t="shared" si="5"/>
-        <v>2.2499999999999964E-2</v>
+        <v>2.1500000000000075E-2</v>
       </c>
       <c r="H21">
         <f t="shared" si="2"/>
-        <v>0.44999999999999929</v>
+        <v>0.43000000000000149</v>
       </c>
       <c r="I21">
         <f t="shared" si="6"/>
-        <v>0.51136363636363558</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+        <v>0.48863636363636531</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="10">
         <v>42355</v>
       </c>
@@ -2054,6 +2054,72 @@
       <c r="I22">
         <f t="shared" si="6"/>
         <v>0.48863636363636531</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="10">
+        <v>42357</v>
+      </c>
+      <c r="B23" s="13">
+        <v>1</v>
+      </c>
+      <c r="C23" s="13">
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="D23" s="13">
+        <v>2.738</v>
+      </c>
+      <c r="E23" s="13">
+        <v>2.7650000000000001</v>
+      </c>
+      <c r="F23" s="13">
+        <f t="shared" si="4"/>
+        <v>2.7565</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="5"/>
+        <v>1.8499999999999961E-2</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="2"/>
+        <v>0.36999999999999922</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="6"/>
+        <v>0.46717171717171618</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="10">
+        <v>42357</v>
+      </c>
+      <c r="B24" s="13">
+        <v>2</v>
+      </c>
+      <c r="C24" s="13">
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="D24" s="13">
+        <v>2.7109999999999999</v>
+      </c>
+      <c r="E24" s="13">
+        <v>2.7389999999999999</v>
+      </c>
+      <c r="F24" s="13">
+        <f t="shared" si="4"/>
+        <v>2.7304999999999997</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="5"/>
+        <v>1.9499999999999851E-2</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="2"/>
+        <v>0.38999999999999702</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="6"/>
+        <v>0.49242424242423866</v>
       </c>
     </row>
   </sheetData>
@@ -2069,21 +2135,21 @@
       <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2097,7 +2163,7 @@
         <v>0.89500000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2138,7 +2204,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2183,7 +2249,7 @@
         <v>0.35999999999997812</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -2232,7 +2298,7 @@
         <v>0.50699999999999967</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -2281,7 +2347,7 @@
         <v>0.60299999999999976</v>
       </c>
     </row>
-    <row r="7" spans="1:16" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>4</v>
       </c>
@@ -2330,7 +2396,7 @@
         <v>0.74800000000000111</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -2378,7 +2444,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -2428,7 +2494,7 @@
         <v>0.48603351955306129</v>
       </c>
     </row>
-    <row r="10" spans="1:16" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -2470,19 +2536,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E13">
         <f>C8-K8</f>
         <v>0.59575000000000244</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="O16">
         <f>AVERAGE(O4:O7)</f>
         <v>0.13080932749067697</v>
       </c>
     </row>
-    <row r="17" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="15:15" ht="15" x14ac:dyDescent="0.25">
       <c r="O17" t="s">
         <v>12</v>
       </c>
@@ -2500,18 +2566,18 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2525,7 +2591,7 @@
         <v>0.91500000000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2566,7 +2632,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2612,7 +2678,7 @@
         <v>0.76000000000000512</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -2662,7 +2728,7 @@
         <v>0.96799999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -2712,7 +2778,7 @@
         <v>2.0679999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:16" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>4</v>
       </c>
@@ -2762,7 +2828,7 @@
         <v>2.8359999999999985</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -2810,7 +2876,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -2860,7 +2926,7 @@
         <v>1.5081967213114742</v>
       </c>
     </row>
-    <row r="10" spans="1:16" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -2915,11 +2981,11 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -3039,12 +3105,12 @@
       <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="10">
         <v>42320</v>
       </c>
@@ -3067,7 +3133,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -3107,7 +3173,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -3154,7 +3220,7 @@
         <v>0.60000000000000053</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3203,7 +3269,7 @@
         <v>0.54999999999998384</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -3241,7 +3307,7 @@
         <v>0.50000000000001155</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -3279,7 +3345,7 @@
         <v>0.44999999999999485</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="F7" t="s">
         <v>40</v>
       </c>
@@ -3302,7 +3368,7 @@
         <v>0.50000000000001155</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="F8" t="s">
         <v>41</v>
       </c>
@@ -3325,7 +3391,7 @@
         <v>0.34999999999998366</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="O9">
         <v>0.69199999999999995</v>
       </c>
@@ -3333,7 +3399,7 @@
         <v>0.45000000000001705</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="10">
         <v>42326</v>
       </c>
@@ -3350,7 +3416,7 @@
         <v>0.44999999999999485</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -3382,7 +3448,7 @@
         <v>0.30000000000001137</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -3411,7 +3477,7 @@
         <v>0.44999999999999485</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2</v>
       </c>
@@ -3440,7 +3506,7 @@
         <v>0.50000000000001155</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>3</v>
       </c>
@@ -3469,7 +3535,7 @@
         <v>0.34999999999998366</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>40</v>
       </c>
@@ -3486,7 +3552,7 @@
         <v>0.43333333333333002</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>41</v>
       </c>
@@ -3503,7 +3569,7 @@
         <v>7.6376261582610933E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:29" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
         <v>42327</v>
       </c>
@@ -3514,7 +3580,7 @@
         <v>0.69199999999999995</v>
       </c>
     </row>
-    <row r="19" spans="1:29" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>36</v>
       </c>
@@ -3534,7 +3600,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" ht="15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -3560,7 +3626,7 @@
         <v>0.45000000000001705</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29" ht="15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2</v>
       </c>
@@ -3586,7 +3652,7 @@
         <v>0.44999999999999485</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29" ht="15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>3</v>
       </c>
@@ -3630,7 +3696,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29" ht="15" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
         <v>46</v>
       </c>
@@ -3667,7 +3733,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:29" ht="15" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
         <v>42</v>
       </c>
@@ -3704,7 +3770,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:29" ht="15" x14ac:dyDescent="0.25">
       <c r="W25" t="s">
         <v>55</v>
       </c>

</xml_diff>